<commit_message>
cleaned and added some inflation rates
</commit_message>
<xml_diff>
--- a/Data/Cataloged_Indicators.xlsx
+++ b/Data/Cataloged_Indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBA2F29-81A6-4D5D-9042-C8474C8BA814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37ACA39-423B-48CE-BCCA-DC14F3A3400D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="91">
   <si>
     <t>Category</t>
   </si>
@@ -281,16 +281,34 @@
     <t>Current Prices, constant PPPs,  (US Dollar, Million, 2015)</t>
   </si>
   <si>
-    <t>32 countries from 2012 + 3 from 2013</t>
-  </si>
-  <si>
-    <t>12 countries from 2012 + 3 from 2013</t>
-  </si>
-  <si>
     <t>~30</t>
   </si>
   <si>
     <t>~65</t>
+  </si>
+  <si>
+    <t>Unemployment Growth QoQ</t>
+  </si>
+  <si>
+    <t>IMF</t>
+  </si>
+  <si>
+    <t>Unemployment Growth YoY</t>
+  </si>
+  <si>
+    <t>OECD, Trading Economics, FX Empire</t>
+  </si>
+  <si>
+    <t>32 countries from 2012 + 3 from 2013, Manually filled</t>
+  </si>
+  <si>
+    <t>12 countries from 2012 + 3 from 2013, Manually filled</t>
+  </si>
+  <si>
+    <t>Combined Yahoo data with csv from Investing</t>
+  </si>
+  <si>
+    <t>Key indicator, manually filled</t>
   </si>
 </sst>
 </file>
@@ -655,7 +673,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,6 +723,9 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="G2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -716,6 +737,9 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
+      <c r="G3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -838,7 +862,47 @@
         <v>98.7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16">
+        <v>98.4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17">
+        <v>96.7</v>
+      </c>
+      <c r="G17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -858,7 +922,7 @@
         <v>68.900000000000006</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>35</v>
       </c>
@@ -875,7 +939,61 @@
         <v>74.599999999999994</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23">
+        <v>84.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24">
+        <v>85.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25">
+        <v>94.3</v>
+      </c>
+      <c r="G25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
@@ -892,7 +1010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>37</v>
       </c>
@@ -909,7 +1027,7 @@
         <v>89.7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>39</v>
       </c>
@@ -926,7 +1044,7 @@
         <v>89.8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>54</v>
       </c>
@@ -943,7 +1061,7 @@
         <v>89.1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>56</v>
       </c>
@@ -960,7 +1078,7 @@
         <v>47.2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>57</v>
       </c>
@@ -977,7 +1095,24 @@
         <v>61.1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" t="s">
+        <v>38</v>
+      </c>
+      <c r="G37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>20</v>
       </c>
@@ -997,7 +1132,7 @@
         <v>94.3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>33</v>
       </c>
@@ -1014,7 +1149,7 @@
         <v>87.7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>34</v>
       </c>
@@ -1031,7 +1166,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>58</v>
       </c>
@@ -1048,7 +1183,7 @@
         <v>63.5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>60</v>
       </c>
@@ -1192,10 +1327,10 @@
         <v>75</v>
       </c>
       <c r="F71" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G71" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -1212,10 +1347,10 @@
         <v>75</v>
       </c>
       <c r="F72" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G72" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
manually filled inflation rates
</commit_message>
<xml_diff>
--- a/Data/Cataloged_Indicators.xlsx
+++ b/Data/Cataloged_Indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37ACA39-423B-48CE-BCCA-DC14F3A3400D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C474B14-C6F5-4B0F-BB50-1AB628F5A88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="92">
   <si>
     <t>Category</t>
   </si>
@@ -281,12 +281,6 @@
     <t>Current Prices, constant PPPs,  (US Dollar, Million, 2015)</t>
   </si>
   <si>
-    <t>~30</t>
-  </si>
-  <si>
-    <t>~65</t>
-  </si>
-  <si>
     <t>Unemployment Growth QoQ</t>
   </si>
   <si>
@@ -308,7 +302,16 @@
     <t>Combined Yahoo data with csv from Investing</t>
   </si>
   <si>
-    <t>Key indicator, manually filled</t>
+    <t>OECD, Trading Economics</t>
+  </si>
+  <si>
+    <t>Key indicator, manually filled missing data</t>
+  </si>
+  <si>
+    <t>35/50</t>
+  </si>
+  <si>
+    <t>15/50</t>
   </si>
 </sst>
 </file>
@@ -673,7 +676,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,7 +727,7 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -738,7 +741,7 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -867,7 +870,7 @@
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -879,7 +882,7 @@
         <v>98.4</v>
       </c>
       <c r="G16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -887,7 +890,7 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
         <v>36</v>
@@ -899,7 +902,7 @@
         <v>96.7</v>
       </c>
       <c r="G17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -941,10 +944,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D23" t="s">
         <v>36</v>
@@ -958,10 +961,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
         <v>36</v>
@@ -978,7 +981,7 @@
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -990,7 +993,7 @@
         <v>94.3</v>
       </c>
       <c r="G25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1100,7 +1103,7 @@
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
         <v>27</v>
@@ -1108,8 +1111,11 @@
       <c r="E37" t="s">
         <v>38</v>
       </c>
+      <c r="F37">
+        <v>99.8</v>
+      </c>
       <c r="G37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1327,10 +1333,10 @@
         <v>75</v>
       </c>
       <c r="F71" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G71" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -1347,10 +1353,10 @@
         <v>75</v>
       </c>
       <c r="F72" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="G72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added World Bank indicators
</commit_message>
<xml_diff>
--- a/Data/Cataloged_Indicators.xlsx
+++ b/Data/Cataloged_Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A933BA-5A0B-43F7-95D7-39F2AC625E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940BE70B-61B1-48C3-B840-1B2C5A771C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="113">
   <si>
     <t>Category</t>
   </si>
@@ -333,6 +333,48 @@
   </si>
   <si>
     <t>Combined Yahoo data with csv imports from Investing</t>
+  </si>
+  <si>
+    <t>World Bank</t>
+  </si>
+  <si>
+    <t>GDP per Capita Current US Dollars</t>
+  </si>
+  <si>
+    <t>Current US Dollar</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Stock Market Cap</t>
+  </si>
+  <si>
+    <t>Current US Dollars</t>
+  </si>
+  <si>
+    <t>Listed domestic companies total</t>
+  </si>
+  <si>
+    <t>Stock Market Cap Pct of GDP</t>
+  </si>
+  <si>
+    <t>Stocks traded total value</t>
+  </si>
+  <si>
+    <t>Stocks traded total value Pct of GDP</t>
+  </si>
+  <si>
+    <t>Current account balance</t>
+  </si>
+  <si>
+    <t>Current account balance US Dollars</t>
+  </si>
+  <si>
+    <t>Government Expense</t>
   </si>
 </sst>
 </file>
@@ -693,11 +735,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BB27A9-49EB-4C78-B689-287C0457C2BE}">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,46 +840,97 @@
         <v>7</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7">
+        <v>77.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8">
+        <v>77.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9">
+        <v>82.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10">
+        <v>79.8</v>
+      </c>
+    </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11">
+        <v>79.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11">
-        <v>94.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12">
-        <v>93.7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>50</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -846,172 +939,189 @@
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="F13">
-        <v>77.2</v>
+        <v>94.7</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="F14">
-        <v>98.7</v>
+        <v>93.7</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F15">
-        <v>98.7</v>
+        <v>77.2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="F16">
-        <v>98.4</v>
-      </c>
-      <c r="G16" t="s">
-        <v>88</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="F17">
-        <v>96.7</v>
-      </c>
-      <c r="G17" t="s">
-        <v>88</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18">
+        <v>98.4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19">
+        <v>96.7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>51</v>
       </c>
-      <c r="C18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
         <v>52</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E20" t="s">
         <v>97</v>
       </c>
-      <c r="F18">
+      <c r="F20">
         <v>98.7</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="F21">
-        <v>68.900000000000006</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
         <v>35</v>
       </c>
-      <c r="C22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" t="s">
         <v>32</v>
       </c>
-      <c r="F22">
-        <v>74.599999999999994</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23">
-        <v>84.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" t="s">
-        <v>38</v>
-      </c>
       <c r="F24">
-        <v>85.6</v>
+        <v>68.900000000000006</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1019,19 +1129,87 @@
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E25" t="s">
         <v>32</v>
       </c>
       <c r="F25">
+        <v>74.599999999999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26">
+        <v>84.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27">
+        <v>85.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28">
         <v>94.3</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G28" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29">
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1156,12 +1334,46 @@
         <v>88</v>
       </c>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39">
+        <v>94.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40">
+        <v>87.7</v>
+      </c>
+    </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C41" t="s">
         <v>26</v>
@@ -1173,12 +1385,12 @@
         <v>32</v>
       </c>
       <c r="F41">
-        <v>94.3</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C42" t="s">
         <v>26</v>
@@ -1187,15 +1399,15 @@
         <v>27</v>
       </c>
       <c r="E42" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="F42">
-        <v>87.7</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C43" t="s">
         <v>26</v>
@@ -1204,268 +1416,458 @@
         <v>27</v>
       </c>
       <c r="E43" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="F43">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>58</v>
-      </c>
-      <c r="C44" t="s">
-        <v>26</v>
-      </c>
-      <c r="D44" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" t="s">
-        <v>59</v>
-      </c>
-      <c r="F44">
         <v>63.5</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B45" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
         <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E45" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="F45">
-        <v>63.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>90.3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46">
+        <v>90.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47">
+        <v>90.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" t="s">
+        <v>62</v>
+      </c>
+      <c r="F48">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" t="s">
+        <v>62</v>
+      </c>
+      <c r="F49">
+        <v>95.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" t="s">
+        <v>62</v>
+      </c>
+      <c r="F50">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
       <c r="C51" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="D51" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="E51" t="s">
         <v>42</v>
       </c>
       <c r="F51">
-        <v>90.3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>93.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
       <c r="C52" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="D52" t="s">
+        <v>52</v>
+      </c>
+      <c r="E52" t="s">
+        <v>105</v>
+      </c>
+      <c r="F52">
+        <v>95.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" t="s">
+        <v>52</v>
+      </c>
+      <c r="E54" t="s">
+        <v>42</v>
+      </c>
+      <c r="F54">
+        <v>69.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" t="s">
+        <v>52</v>
+      </c>
+      <c r="E55" t="s">
+        <v>95</v>
+      </c>
+      <c r="F55">
+        <v>79.099999999999994</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" t="s">
+        <v>52</v>
+      </c>
+      <c r="E56" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56">
+        <v>79.099999999999994</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" t="s">
+        <v>42</v>
+      </c>
+      <c r="F57">
+        <v>79.099999999999994</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" t="s">
+        <v>52</v>
+      </c>
+      <c r="E58" t="s">
+        <v>42</v>
+      </c>
+      <c r="F58">
+        <v>79.400000000000006</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" t="s">
+        <v>77</v>
+      </c>
+      <c r="D60" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F60" t="s">
+        <v>89</v>
+      </c>
+      <c r="G60" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" t="s">
+        <v>75</v>
+      </c>
+      <c r="F61" t="s">
+        <v>90</v>
+      </c>
+      <c r="G61" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" t="s">
+        <v>28</v>
+      </c>
+      <c r="F62">
+        <v>93.3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>30</v>
+      </c>
+      <c r="C63" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" t="s">
+        <v>28</v>
+      </c>
+      <c r="F63">
+        <v>43.6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>43</v>
+      </c>
+      <c r="C64" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" t="s">
+        <v>38</v>
+      </c>
+      <c r="F64">
+        <v>77.7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65" t="s">
+        <v>26</v>
+      </c>
+      <c r="D65" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" t="s">
+        <v>66</v>
+      </c>
+      <c r="F65">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E66" t="s">
+        <v>66</v>
+      </c>
+      <c r="F66">
+        <v>77.3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" t="s">
+        <v>27</v>
+      </c>
+      <c r="E67" t="s">
+        <v>66</v>
+      </c>
+      <c r="F67">
+        <v>57.3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B69" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" t="s">
+        <v>26</v>
+      </c>
+      <c r="D69" t="s">
+        <v>27</v>
+      </c>
+      <c r="E69" t="s">
+        <v>28</v>
+      </c>
+      <c r="F69">
+        <v>84.7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>44</v>
+      </c>
+      <c r="C70" t="s">
+        <v>26</v>
+      </c>
+      <c r="D70" t="s">
         <v>36</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E70" t="s">
         <v>38</v>
       </c>
-      <c r="F52">
-        <v>90.2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>49</v>
-      </c>
-      <c r="C53" t="s">
-        <v>26</v>
-      </c>
-      <c r="D53" t="s">
-        <v>36</v>
-      </c>
-      <c r="E53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F53">
-        <v>90.2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>61</v>
-      </c>
-      <c r="C54" t="s">
-        <v>26</v>
-      </c>
-      <c r="D54" t="s">
-        <v>27</v>
-      </c>
-      <c r="E54" t="s">
-        <v>62</v>
-      </c>
-      <c r="F54">
-        <v>95.5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" t="s">
-        <v>26</v>
-      </c>
-      <c r="D55" t="s">
-        <v>27</v>
-      </c>
-      <c r="E55" t="s">
-        <v>62</v>
-      </c>
-      <c r="F55">
-        <v>95.7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>64</v>
-      </c>
-      <c r="C56" t="s">
-        <v>26</v>
-      </c>
-      <c r="D56" t="s">
-        <v>27</v>
-      </c>
-      <c r="E56" t="s">
-        <v>62</v>
-      </c>
-      <c r="F56">
-        <v>95.5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B61" t="s">
-        <v>91</v>
-      </c>
-      <c r="C61" t="s">
-        <v>26</v>
-      </c>
-      <c r="D61" t="s">
-        <v>52</v>
-      </c>
-      <c r="E61" t="s">
-        <v>42</v>
-      </c>
-      <c r="F61">
-        <v>69.8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>92</v>
-      </c>
-      <c r="C62" t="s">
-        <v>26</v>
-      </c>
-      <c r="D62" t="s">
-        <v>52</v>
-      </c>
-      <c r="E62" t="s">
-        <v>95</v>
-      </c>
-      <c r="F62">
-        <v>79.099999999999994</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>93</v>
-      </c>
-      <c r="C63" t="s">
-        <v>26</v>
-      </c>
-      <c r="D63" t="s">
-        <v>52</v>
-      </c>
-      <c r="E63" t="s">
-        <v>95</v>
-      </c>
-      <c r="F63">
-        <v>79.099999999999994</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>94</v>
-      </c>
-      <c r="C64" t="s">
-        <v>26</v>
-      </c>
-      <c r="D64" t="s">
-        <v>52</v>
-      </c>
-      <c r="E64" t="s">
-        <v>42</v>
-      </c>
-      <c r="F64">
-        <v>79.099999999999994</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="F70">
+        <v>86.9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C71" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="D71" t="s">
         <v>27</v>
       </c>
       <c r="E71" t="s">
-        <v>75</v>
-      </c>
-      <c r="F71" t="s">
-        <v>89</v>
-      </c>
-      <c r="G71" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="F71">
+        <v>67.599999999999994</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C72" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="D72" t="s">
         <v>27</v>
       </c>
       <c r="E72" t="s">
-        <v>75</v>
-      </c>
-      <c r="F72" t="s">
-        <v>90</v>
-      </c>
-      <c r="G72" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="F72">
+        <v>62.3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="C73" t="s">
         <v>26</v>
@@ -1474,186 +1876,14 @@
         <v>27</v>
       </c>
       <c r="E73" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="F73">
-        <v>93.3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>30</v>
-      </c>
-      <c r="C74" t="s">
-        <v>26</v>
-      </c>
-      <c r="D74" t="s">
-        <v>27</v>
-      </c>
-      <c r="E74" t="s">
-        <v>28</v>
-      </c>
-      <c r="F74">
-        <v>43.6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>43</v>
-      </c>
-      <c r="C75" t="s">
-        <v>26</v>
-      </c>
-      <c r="D75" t="s">
-        <v>27</v>
-      </c>
-      <c r="E75" t="s">
-        <v>38</v>
-      </c>
-      <c r="F75">
-        <v>77.7</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>69</v>
-      </c>
-      <c r="C76" t="s">
-        <v>26</v>
-      </c>
-      <c r="D76" t="s">
-        <v>27</v>
-      </c>
-      <c r="E76" t="s">
-        <v>66</v>
-      </c>
-      <c r="F76">
-        <v>85.5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>70</v>
-      </c>
-      <c r="C77" t="s">
-        <v>26</v>
-      </c>
-      <c r="D77" t="s">
-        <v>27</v>
-      </c>
-      <c r="E77" t="s">
-        <v>66</v>
-      </c>
-      <c r="F77">
-        <v>77.3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>71</v>
-      </c>
-      <c r="C78" t="s">
-        <v>26</v>
-      </c>
-      <c r="D78" t="s">
-        <v>27</v>
-      </c>
-      <c r="E78" t="s">
-        <v>66</v>
-      </c>
-      <c r="F78">
-        <v>57.3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B81" t="s">
-        <v>29</v>
-      </c>
-      <c r="C81" t="s">
-        <v>26</v>
-      </c>
-      <c r="D81" t="s">
-        <v>27</v>
-      </c>
-      <c r="E81" t="s">
-        <v>28</v>
-      </c>
-      <c r="F81">
-        <v>84.7</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>44</v>
-      </c>
-      <c r="C82" t="s">
-        <v>26</v>
-      </c>
-      <c r="D82" t="s">
-        <v>36</v>
-      </c>
-      <c r="E82" t="s">
-        <v>38</v>
-      </c>
-      <c r="F82">
-        <v>86.9</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>65</v>
-      </c>
-      <c r="C83" t="s">
-        <v>26</v>
-      </c>
-      <c r="D83" t="s">
-        <v>27</v>
-      </c>
-      <c r="E83" t="s">
-        <v>66</v>
-      </c>
-      <c r="F83">
-        <v>67.599999999999994</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>67</v>
-      </c>
-      <c r="C84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D84" t="s">
-        <v>27</v>
-      </c>
-      <c r="E84" t="s">
-        <v>66</v>
-      </c>
-      <c r="F84">
-        <v>62.3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>68</v>
-      </c>
-      <c r="C85" t="s">
-        <v>26</v>
-      </c>
-      <c r="D85" t="s">
-        <v>27</v>
-      </c>
-      <c r="E85" t="s">
-        <v>66</v>
-      </c>
-      <c r="F85">
         <v>54.7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added inventories and extra notes to investments
</commit_message>
<xml_diff>
--- a/Data/Cataloged_Indicators.xlsx
+++ b/Data/Cataloged_Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940BE70B-61B1-48C3-B840-1B2C5A771C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0AABDE-286A-4F9D-BF99-62CF771C2A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="114">
   <si>
     <t>Category</t>
   </si>
@@ -375,6 +375,9 @@
   </si>
   <si>
     <t>Government Expense</t>
+  </si>
+  <si>
+    <t>Changes in inventories</t>
   </si>
 </sst>
 </file>
@@ -735,11 +738,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BB27A9-49EB-4C78-B689-287C0457C2BE}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,63 +1797,63 @@
         <v>57.3</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>113</v>
+      </c>
+      <c r="C68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" t="s">
+        <v>36</v>
+      </c>
+      <c r="E68" t="s">
+        <v>95</v>
+      </c>
+      <c r="F68">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>29</v>
       </c>
-      <c r="C69" t="s">
-        <v>26</v>
-      </c>
-      <c r="D69" t="s">
-        <v>27</v>
-      </c>
-      <c r="E69" t="s">
+      <c r="C70" t="s">
+        <v>26</v>
+      </c>
+      <c r="D70" t="s">
+        <v>27</v>
+      </c>
+      <c r="E70" t="s">
         <v>28</v>
       </c>
-      <c r="F69">
+      <c r="F70">
         <v>84.7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>44</v>
-      </c>
-      <c r="C70" t="s">
-        <v>26</v>
-      </c>
-      <c r="D70" t="s">
-        <v>36</v>
-      </c>
-      <c r="E70" t="s">
-        <v>38</v>
-      </c>
-      <c r="F70">
-        <v>86.9</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C71" t="s">
         <v>26</v>
       </c>
       <c r="D71" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E71" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="F71">
-        <v>67.599999999999994</v>
+        <v>86.9</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C72" t="s">
         <v>26</v>
@@ -1862,12 +1865,12 @@
         <v>66</v>
       </c>
       <c r="F72">
-        <v>62.3</v>
+        <v>67.599999999999994</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C73" t="s">
         <v>26</v>
@@ -1879,6 +1882,23 @@
         <v>66</v>
       </c>
       <c r="F73">
+        <v>62.3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>68</v>
+      </c>
+      <c r="C74" t="s">
+        <v>26</v>
+      </c>
+      <c r="D74" t="s">
+        <v>27</v>
+      </c>
+      <c r="E74" t="s">
+        <v>66</v>
+      </c>
+      <c r="F74">
         <v>54.7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
db setup and semi-automatic web scrapping
</commit_message>
<xml_diff>
--- a/Data/Cataloged_Indicators.xlsx
+++ b/Data/Cataloged_Indicators.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0AABDE-286A-4F9D-BF99-62CF771C2A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30CB591-5A5D-4CB9-A689-DB102A75F68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
   </bookViews>
@@ -741,8 +741,8 @@
   <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated remaining oecd indicators
</commit_message>
<xml_diff>
--- a/Data/Cataloged_Indicators.xlsx
+++ b/Data/Cataloged_Indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F4797E-17F0-4184-9553-F75F7A02CA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6460A6-0A00-422A-8E45-B9F7DF4239B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicators" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="131">
   <si>
     <t>Category</t>
   </si>
@@ -188,9 +188,6 @@
     <t>GDP per capita</t>
   </si>
   <si>
-    <t>GDP Current Prices</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -296,9 +293,6 @@
     <t>12 countries from 2012 + 3 from 2013, Manually filled</t>
   </si>
   <si>
-    <t>OECD, Trading Economics</t>
-  </si>
-  <si>
     <t>Key indicator, manually filled missing data</t>
   </si>
   <si>
@@ -324,9 +318,6 @@
   </si>
   <si>
     <t>GDP Current Prices US Dollars</t>
-  </si>
-  <si>
-    <t>Current Prices, local currency</t>
   </si>
   <si>
     <t>Combined Yahoo data with csv imports from Investing</t>
@@ -802,7 +793,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,10 +825,10 @@
         <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -857,7 +848,7 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -871,7 +862,7 @@
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -909,16 +900,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F7">
         <v>77.8</v>
@@ -926,13 +917,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
         <v>41</v>
@@ -943,16 +934,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F9">
         <v>82.1</v>
@@ -960,16 +951,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F10">
         <v>79.8</v>
@@ -977,13 +968,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
         <v>41</v>
@@ -1009,7 +1000,10 @@
         <v>37</v>
       </c>
       <c r="F13">
-        <v>94.7</v>
+        <v>73.900000000000006</v>
+      </c>
+      <c r="G13">
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1026,7 +1020,10 @@
         <v>46</v>
       </c>
       <c r="F14">
-        <v>93.7</v>
+        <v>73.099999999999994</v>
+      </c>
+      <c r="G14">
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1040,44 +1037,53 @@
         <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F15">
-        <v>77.2</v>
+        <v>60.1</v>
+      </c>
+      <c r="G15">
+        <v>74.5</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16">
-        <v>98.7</v>
+        <v>77</v>
+      </c>
+      <c r="G16">
+        <v>94.3</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F17">
-        <v>98.7</v>
+        <v>77</v>
+      </c>
+      <c r="G17">
+        <v>94.3</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1085,7 +1091,7 @@
         <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
         <v>35</v>
@@ -1093,11 +1099,11 @@
       <c r="E18" t="s">
         <v>37</v>
       </c>
-      <c r="F18">
-        <v>98.4</v>
+      <c r="G18">
+        <v>99.9</v>
       </c>
       <c r="H18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1105,7 +1111,7 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
         <v>35</v>
@@ -1113,42 +1119,42 @@
       <c r="E19" t="s">
         <v>46</v>
       </c>
-      <c r="F19">
-        <v>96.7</v>
+      <c r="G19">
+        <v>99.3</v>
       </c>
       <c r="H19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" t="s">
         <v>50</v>
       </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" t="s">
-        <v>51</v>
-      </c>
       <c r="E20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F20">
-        <v>98.7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" t="s">
         <v>95</v>
       </c>
-      <c r="C21" t="s">
-        <v>98</v>
-      </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F21">
         <v>100</v>
@@ -1156,65 +1162,68 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="F22">
-        <v>100</v>
+        <v>36</v>
+      </c>
+      <c r="G22">
+        <v>76.099999999999994</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D23" t="s">
         <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F23">
-        <v>36</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="G23">
-        <v>76.099999999999994</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C24" t="s">
-        <v>133</v>
-      </c>
-      <c r="D24" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24">
-        <v>37.700000000000003</v>
-      </c>
-      <c r="G24">
         <v>73.599999999999994</v>
       </c>
     </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25">
+        <v>53.6</v>
+      </c>
+      <c r="G25">
+        <v>66.099999999999994</v>
+      </c>
+    </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="B26" t="s">
         <v>34</v>
       </c>
@@ -1222,138 +1231,144 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
         <v>31</v>
       </c>
       <c r="F26">
-        <v>68.900000000000006</v>
+        <v>58.2</v>
+      </c>
+      <c r="G26">
+        <v>69.8</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="D27" t="s">
         <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="F27">
-        <v>74.599999999999994</v>
+        <v>84.3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
         <v>80</v>
-      </c>
-      <c r="C28" t="s">
-        <v>81</v>
       </c>
       <c r="D28" t="s">
         <v>35</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F28">
-        <v>84.3</v>
+        <v>85.6</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
         <v>82</v>
       </c>
-      <c r="C29" t="s">
-        <v>81</v>
-      </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E29" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29">
-        <v>85.6</v>
+        <v>31</v>
+      </c>
+      <c r="G29">
+        <v>88.1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="E30" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="F30">
-        <v>94.3</v>
-      </c>
-      <c r="H30" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="D31" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="E31" t="s">
-        <v>102</v>
+        <v>31</v>
       </c>
       <c r="F31">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" t="s">
-        <v>133</v>
-      </c>
-      <c r="D32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" t="s">
+        <v>53.1</v>
+      </c>
+      <c r="G31">
+        <v>64.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
         <v>31</v>
       </c>
-      <c r="F32">
-        <v>53.1</v>
-      </c>
-      <c r="G32">
-        <v>64.2</v>
-      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E34" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="F34">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="G34">
+        <v>91.1</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1364,13 +1379,16 @@
         <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E35" t="s">
         <v>37</v>
       </c>
       <c r="F35">
-        <v>89.7</v>
+        <v>74.2</v>
+      </c>
+      <c r="G35">
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1387,29 +1405,35 @@
         <v>39</v>
       </c>
       <c r="F36">
-        <v>89.8</v>
+        <v>70</v>
+      </c>
+      <c r="G36">
+        <v>90.3</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" t="s">
         <v>53</v>
       </c>
-      <c r="C37" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" t="s">
-        <v>26</v>
-      </c>
-      <c r="E37" t="s">
-        <v>54</v>
-      </c>
       <c r="F37">
-        <v>89.1</v>
+        <v>69.5</v>
+      </c>
+      <c r="G37">
+        <v>88.2</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
         <v>25</v>
@@ -1418,15 +1442,18 @@
         <v>26</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F38">
-        <v>47.2</v>
+        <v>36.799999999999997</v>
+      </c>
+      <c r="G38">
+        <v>41.8</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
         <v>25</v>
@@ -1435,10 +1462,13 @@
         <v>26</v>
       </c>
       <c r="E39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F39">
-        <v>61.1</v>
+        <v>47.7</v>
+      </c>
+      <c r="G39">
+        <v>52.5</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1446,7 +1476,7 @@
         <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D40" t="s">
         <v>26</v>
@@ -1454,19 +1484,19 @@
       <c r="E40" t="s">
         <v>37</v>
       </c>
-      <c r="F40">
-        <v>99.8</v>
+      <c r="G40">
+        <v>97.2</v>
       </c>
       <c r="H40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D41" t="s">
         <v>26</v>
@@ -1483,10 +1513,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D42" t="s">
         <v>26</v>
@@ -1503,10 +1533,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D43" t="s">
         <v>26</v>
@@ -1523,10 +1553,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C44" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D44" t="s">
         <v>26</v>
@@ -1543,10 +1573,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" t="s">
         <v>130</v>
-      </c>
-      <c r="C45" t="s">
-        <v>133</v>
       </c>
       <c r="D45" t="s">
         <v>26</v>
@@ -1563,10 +1593,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C46" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D46" t="s">
         <v>26</v>
@@ -1598,7 +1628,10 @@
         <v>31</v>
       </c>
       <c r="F48">
-        <v>94.3</v>
+        <v>73.7</v>
+      </c>
+      <c r="G48">
+        <v>88.7</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1615,7 +1648,10 @@
         <v>31</v>
       </c>
       <c r="F49">
-        <v>87.7</v>
+        <v>68.400000000000006</v>
+      </c>
+      <c r="G49">
+        <v>82.6</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1632,29 +1668,35 @@
         <v>31</v>
       </c>
       <c r="F50">
-        <v>85</v>
+        <v>66.400000000000006</v>
+      </c>
+      <c r="G50">
+        <v>83.6</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" t="s">
         <v>57</v>
       </c>
-      <c r="C51" t="s">
-        <v>25</v>
-      </c>
-      <c r="D51" t="s">
-        <v>26</v>
-      </c>
-      <c r="E51" t="s">
-        <v>58</v>
-      </c>
       <c r="F51">
-        <v>63.5</v>
+        <v>49.5</v>
+      </c>
+      <c r="G51">
+        <v>62.9</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C52" t="s">
         <v>25</v>
@@ -1663,10 +1705,13 @@
         <v>26</v>
       </c>
       <c r="E52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F52">
-        <v>63.5</v>
+        <v>49.5</v>
+      </c>
+      <c r="G52">
+        <v>62.9</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1686,7 +1731,10 @@
         <v>41</v>
       </c>
       <c r="F54">
-        <v>90.3</v>
+        <v>70</v>
+      </c>
+      <c r="G54">
+        <v>94.4</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1703,7 +1751,10 @@
         <v>37</v>
       </c>
       <c r="F55">
-        <v>90.2</v>
+        <v>70.3</v>
+      </c>
+      <c r="G55">
+        <v>89.1</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -1720,29 +1771,35 @@
         <v>37</v>
       </c>
       <c r="F56">
-        <v>90.2</v>
+        <v>70.3</v>
+      </c>
+      <c r="G56">
+        <v>89.1</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57" t="s">
         <v>60</v>
       </c>
-      <c r="C57" t="s">
-        <v>25</v>
-      </c>
-      <c r="D57" t="s">
-        <v>26</v>
-      </c>
-      <c r="E57" t="s">
-        <v>61</v>
-      </c>
       <c r="F57">
-        <v>95.5</v>
+        <v>74.2</v>
+      </c>
+      <c r="G57">
+        <v>94.6</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" t="s">
         <v>25</v>
@@ -1751,15 +1808,18 @@
         <v>26</v>
       </c>
       <c r="E58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F58">
-        <v>95.7</v>
+        <v>74.400000000000006</v>
+      </c>
+      <c r="G58">
+        <v>95.3</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s">
         <v>25</v>
@@ -1768,21 +1828,24 @@
         <v>26</v>
       </c>
       <c r="E59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F59">
-        <v>95.5</v>
+        <v>74.2</v>
+      </c>
+      <c r="G59">
+        <v>94.6</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C60" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E60" t="s">
         <v>41</v>
@@ -1793,16 +1856,16 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C61" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E61" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F61">
         <v>95.2</v>
@@ -1810,16 +1873,16 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C62" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D62" t="s">
         <v>26</v>
       </c>
       <c r="E62" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F62">
         <v>64.900000000000006</v>
@@ -1830,16 +1893,16 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C63" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D63" t="s">
         <v>26</v>
       </c>
       <c r="E63" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F63">
         <v>10.5</v>
@@ -1853,87 +1916,96 @@
         <v>21</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C65" t="s">
         <v>25</v>
       </c>
       <c r="D65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E65" t="s">
         <v>41</v>
       </c>
       <c r="F65">
-        <v>69.8</v>
+        <v>54.8</v>
+      </c>
+      <c r="G65">
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C66" t="s">
         <v>25</v>
       </c>
       <c r="D66" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E66" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F66">
-        <v>79.099999999999994</v>
+        <v>61.9</v>
+      </c>
+      <c r="G66">
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" t="s">
+        <v>25</v>
+      </c>
+      <c r="D67" t="s">
+        <v>50</v>
+      </c>
+      <c r="E67" t="s">
         <v>92</v>
       </c>
-      <c r="C67" t="s">
-        <v>25</v>
-      </c>
-      <c r="D67" t="s">
-        <v>51</v>
-      </c>
-      <c r="E67" t="s">
-        <v>94</v>
-      </c>
       <c r="F67">
-        <v>79.099999999999994</v>
+        <v>61.9</v>
+      </c>
+      <c r="G67">
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C68" t="s">
         <v>25</v>
       </c>
       <c r="D68" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E68" t="s">
         <v>41</v>
       </c>
       <c r="F68">
-        <v>79.099999999999994</v>
+        <v>77</v>
+      </c>
+      <c r="G68">
+        <v>94.3</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C69" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D69" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E69" t="s">
         <v>41</v>
-      </c>
-      <c r="F69">
-        <v>79.400000000000006</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -1941,42 +2013,42 @@
         <v>22</v>
       </c>
       <c r="B71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C71" t="s">
+        <v>75</v>
+      </c>
+      <c r="D71" t="s">
+        <v>26</v>
+      </c>
+      <c r="E71" t="s">
         <v>73</v>
       </c>
-      <c r="C71" t="s">
-        <v>76</v>
-      </c>
-      <c r="D71" t="s">
-        <v>26</v>
-      </c>
-      <c r="E71" t="s">
-        <v>74</v>
-      </c>
       <c r="F71" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
+        <v>74</v>
+      </c>
+      <c r="C72" t="s">
         <v>75</v>
       </c>
-      <c r="C72" t="s">
-        <v>76</v>
-      </c>
       <c r="D72" t="s">
         <v>26</v>
       </c>
       <c r="E72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F72" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H72" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -1993,7 +2065,10 @@
         <v>27</v>
       </c>
       <c r="F73">
-        <v>93.3</v>
+        <v>72.7</v>
+      </c>
+      <c r="G73">
+        <v>88.5</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -2010,7 +2085,10 @@
         <v>27</v>
       </c>
       <c r="F74">
-        <v>43.6</v>
+        <v>34</v>
+      </c>
+      <c r="G74">
+        <v>56.7</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -2027,12 +2105,15 @@
         <v>37</v>
       </c>
       <c r="F75">
-        <v>77.7</v>
+        <v>60.6</v>
+      </c>
+      <c r="G75">
+        <v>72.099999999999994</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C76" t="s">
         <v>25</v>
@@ -2041,15 +2122,18 @@
         <v>26</v>
       </c>
       <c r="E76" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F76">
-        <v>85.5</v>
+        <v>66.7</v>
+      </c>
+      <c r="G76">
+        <v>82.1</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C77" t="s">
         <v>25</v>
@@ -2058,15 +2142,18 @@
         <v>26</v>
       </c>
       <c r="E77" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F77">
-        <v>77.3</v>
+        <v>60.3</v>
+      </c>
+      <c r="G77">
+        <v>70.5</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C78" t="s">
         <v>25</v>
@@ -2075,15 +2162,18 @@
         <v>26</v>
       </c>
       <c r="E78" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F78">
-        <v>57.3</v>
+        <v>44.7</v>
+      </c>
+      <c r="G78">
+        <v>56.4</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C79" t="s">
         <v>25</v>
@@ -2092,24 +2182,27 @@
         <v>35</v>
       </c>
       <c r="E79" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F79">
-        <v>80</v>
+        <v>62.3</v>
+      </c>
+      <c r="G79">
+        <v>82.6</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
+        <v>72</v>
+      </c>
+      <c r="C80" t="s">
+        <v>130</v>
+      </c>
+      <c r="D80" t="s">
+        <v>26</v>
+      </c>
+      <c r="E80" t="s">
         <v>73</v>
-      </c>
-      <c r="C80" t="s">
-        <v>133</v>
-      </c>
-      <c r="D80" t="s">
-        <v>26</v>
-      </c>
-      <c r="E80" t="s">
-        <v>74</v>
       </c>
       <c r="F80">
         <v>31.8</v>
@@ -2120,16 +2213,16 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C81" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D81" t="s">
         <v>26</v>
       </c>
       <c r="E81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F81">
         <v>14.6</v>
@@ -2140,16 +2233,16 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C82" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D82" t="s">
         <v>26</v>
       </c>
       <c r="E82" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F82">
         <v>7.2</v>
@@ -2160,16 +2253,16 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C83" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D83" t="s">
         <v>26</v>
       </c>
       <c r="E83" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F83">
         <v>1.9</v>
@@ -2180,10 +2273,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C84" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D84" t="s">
         <v>26</v>
@@ -2200,10 +2293,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C85" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D85" t="s">
         <v>26</v>
@@ -2235,7 +2328,10 @@
         <v>27</v>
       </c>
       <c r="F87">
-        <v>84.7</v>
+        <v>66.099999999999994</v>
+      </c>
+      <c r="G87">
+        <v>81.8</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -2252,29 +2348,35 @@
         <v>37</v>
       </c>
       <c r="F88">
-        <v>86.9</v>
+        <v>67.7</v>
+      </c>
+      <c r="G88">
+        <v>85.9</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
+        <v>63</v>
+      </c>
+      <c r="C89" t="s">
+        <v>25</v>
+      </c>
+      <c r="D89" t="s">
+        <v>26</v>
+      </c>
+      <c r="E89" t="s">
         <v>64</v>
       </c>
-      <c r="C89" t="s">
-        <v>25</v>
-      </c>
-      <c r="D89" t="s">
-        <v>26</v>
-      </c>
-      <c r="E89" t="s">
-        <v>65</v>
-      </c>
       <c r="F89">
-        <v>67.599999999999994</v>
+        <v>52.7</v>
+      </c>
+      <c r="G89">
+        <v>59.8</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C90" t="s">
         <v>25</v>
@@ -2283,15 +2385,18 @@
         <v>26</v>
       </c>
       <c r="E90" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F90">
-        <v>62.3</v>
+        <v>48.4</v>
+      </c>
+      <c r="G90">
+        <v>53.3</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C91" t="s">
         <v>25</v>
@@ -2300,18 +2405,21 @@
         <v>26</v>
       </c>
       <c r="E91" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F91">
-        <v>54.7</v>
+        <v>42.6</v>
+      </c>
+      <c r="G91">
+        <v>41.8</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C92" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D92" t="s">
         <v>26</v>
@@ -2328,10 +2436,10 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C93" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D93" t="s">
         <v>26</v>
@@ -2348,16 +2456,16 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C94" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D94" t="s">
         <v>26</v>
       </c>
       <c r="E94" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F94">
         <v>33.9</v>

</xml_diff>

<commit_message>
updated countries on economic calendar
</commit_message>
<xml_diff>
--- a/Data/Cataloged_Indicators.xlsx
+++ b/Data/Cataloged_Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6460A6-0A00-422A-8E45-B9F7DF4239B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA31F7E-DD1C-438B-A29C-88CF38C78C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
   </bookViews>
@@ -793,7 +793,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1528,7 +1528,7 @@
         <v>79.3</v>
       </c>
       <c r="G42">
-        <v>85</v>
+        <v>85.1</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated world bank indicators
</commit_message>
<xml_diff>
--- a/Data/Cataloged_Indicators.xlsx
+++ b/Data/Cataloged_Indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA31F7E-DD1C-438B-A29C-88CF38C78C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6443D0-3A94-4F9D-88B0-597A58D12025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="536" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicators" sheetId="1" r:id="rId1"/>
@@ -792,8 +792,8 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,7 +912,10 @@
         <v>101</v>
       </c>
       <c r="F7">
-        <v>77.8</v>
+        <v>76.2</v>
+      </c>
+      <c r="G7">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -929,7 +932,10 @@
         <v>41</v>
       </c>
       <c r="F8">
-        <v>77.8</v>
+        <v>76.2</v>
+      </c>
+      <c r="G8">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -946,7 +952,10 @@
         <v>99</v>
       </c>
       <c r="F9">
-        <v>82.1</v>
+        <v>80.5</v>
+      </c>
+      <c r="G9">
+        <v>65.7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -963,7 +972,10 @@
         <v>101</v>
       </c>
       <c r="F10">
-        <v>79.8</v>
+        <v>78.2</v>
+      </c>
+      <c r="G10">
+        <v>63.7</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -980,7 +992,10 @@
         <v>41</v>
       </c>
       <c r="F11">
-        <v>79.8</v>
+        <v>78.2</v>
+      </c>
+      <c r="G11">
+        <v>63.7</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1140,7 +1155,10 @@
         <v>97</v>
       </c>
       <c r="F20">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="G20">
+        <v>96.7</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1157,7 +1175,10 @@
         <v>97</v>
       </c>
       <c r="F21">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="G21">
+        <v>96.7</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1311,7 +1332,10 @@
         <v>99</v>
       </c>
       <c r="F30">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="G30">
+        <v>96.7</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1851,7 +1875,10 @@
         <v>41</v>
       </c>
       <c r="F60">
-        <v>93.3</v>
+        <v>91.4</v>
+      </c>
+      <c r="G60">
+        <v>96.3</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -1868,7 +1895,10 @@
         <v>101</v>
       </c>
       <c r="F61">
-        <v>95.2</v>
+        <v>93.3</v>
+      </c>
+      <c r="G61">
+        <v>96.3</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2006,6 +2036,12 @@
       </c>
       <c r="E69" t="s">
         <v>41</v>
+      </c>
+      <c r="F69">
+        <v>77.8</v>
+      </c>
+      <c r="G69">
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
saved all oecd indicators to db
</commit_message>
<xml_diff>
--- a/Data/Cataloged_Indicators.xlsx
+++ b/Data/Cataloged_Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11DE8E1-4607-424F-8683-2D5D1DED7100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639FDB92-8CDA-47B0-9D08-D932B2906680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="536" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="132">
   <si>
     <t>Category</t>
   </si>
@@ -125,21 +125,12 @@
     <t>OECD Consumer Confidence Indicator</t>
   </si>
   <si>
-    <t>Composite Leading Indicators</t>
-  </si>
-  <si>
     <t>Overnight Interbank Rate</t>
   </si>
   <si>
     <t>Level</t>
   </si>
   <si>
-    <t>Short term interest rate</t>
-  </si>
-  <si>
-    <t>Long term interest rate</t>
-  </si>
-  <si>
     <t>Unemployment Rate</t>
   </si>
   <si>
@@ -185,18 +176,12 @@
     <t>Import of goods and services</t>
   </si>
   <si>
-    <t>GDP per capita</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
     <t>GDP Current Prices PPP</t>
   </si>
   <si>
-    <t>Customer Price Index - All Items Total</t>
-  </si>
-  <si>
     <t>Index 2015 = 100</t>
   </si>
   <si>
@@ -206,15 +191,9 @@
     <t>PPI Manufacturing</t>
   </si>
   <si>
-    <t>Narrow Money - M1 and components</t>
-  </si>
-  <si>
     <t>National Currency</t>
   </si>
   <si>
-    <t>Broad Money - M3 and components</t>
-  </si>
-  <si>
     <t>Export - Value (goods)</t>
   </si>
   <si>
@@ -227,27 +206,12 @@
     <t>Net Trade - Value (goods)</t>
   </si>
   <si>
-    <t>Total retail sales value</t>
-  </si>
-  <si>
     <t>Index 2015=100, s.a.</t>
   </si>
   <si>
     <t>Passenger Car Registration</t>
   </si>
   <si>
-    <t>Permits issued - Residential Buildings</t>
-  </si>
-  <si>
-    <t>Total manufacturing</t>
-  </si>
-  <si>
-    <t>Total industry ex construction</t>
-  </si>
-  <si>
-    <t>Total construction</t>
-  </si>
-  <si>
     <t>Central Bank Rates</t>
   </si>
   <si>
@@ -269,9 +233,6 @@
     <t>Per Head, US dollars (2015), fixed PPPs, s. a.</t>
   </si>
   <si>
-    <t>Current Prices, constant exchange rate,(US Dollar, Million, 2015)</t>
-  </si>
-  <si>
     <t>Current Prices, constant PPPs,  (US Dollar, Million, 2015)</t>
   </si>
   <si>
@@ -365,9 +326,6 @@
     <t>Government Expense</t>
   </si>
   <si>
-    <t>Changes in inventories</t>
-  </si>
-  <si>
     <t>GDP (YoY)</t>
   </si>
   <si>
@@ -429,6 +387,51 @@
   </si>
   <si>
     <t>Investing Economic Calendar</t>
+  </si>
+  <si>
+    <t>GDP Per Capita</t>
+  </si>
+  <si>
+    <t>Current Prices, constant exchange rate, (US Dollar, Million, 2015)</t>
+  </si>
+  <si>
+    <t>CPI</t>
+  </si>
+  <si>
+    <t>Short Term Interest Rate</t>
+  </si>
+  <si>
+    <t>Long Term Interest Rate</t>
+  </si>
+  <si>
+    <t>Narrow Money M1</t>
+  </si>
+  <si>
+    <t>Broad Money M3</t>
+  </si>
+  <si>
+    <t>OECD Composite Leading Indicators</t>
+  </si>
+  <si>
+    <t>Total Manufacturing</t>
+  </si>
+  <si>
+    <t>Total Industry ex Construction</t>
+  </si>
+  <si>
+    <t>Total Construction</t>
+  </si>
+  <si>
+    <t>Changes in Inventories</t>
+  </si>
+  <si>
+    <t>Total Retail Sales Value</t>
+  </si>
+  <si>
+    <t>Permits Issued (Residential Buildings)</t>
+  </si>
+  <si>
+    <t>Calculated</t>
   </si>
 </sst>
 </file>
@@ -792,8 +795,8 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H92" sqref="H92"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,10 +828,10 @@
         <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -848,7 +851,7 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -862,7 +865,7 @@
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -900,16 +903,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="F7">
         <v>76.2</v>
@@ -920,16 +923,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F8">
         <v>76.2</v>
@@ -940,16 +943,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="F9">
         <v>80.5</v>
@@ -960,16 +963,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="F10">
         <v>78.2</v>
@@ -980,16 +983,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F11">
         <v>78.2</v>
@@ -1003,16 +1006,16 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F13">
         <v>73.900000000000006</v>
@@ -1023,16 +1026,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F14">
         <v>73.099999999999994</v>
@@ -1043,16 +1046,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F15">
         <v>60.1</v>
@@ -1063,16 +1066,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="F16">
         <v>77</v>
@@ -1083,16 +1086,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="F17">
         <v>77</v>
@@ -1103,56 +1106,56 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G18">
         <v>99.9</v>
       </c>
       <c r="H18" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G19">
         <v>99.3</v>
       </c>
       <c r="H19" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="F20">
         <v>98</v>
@@ -1163,16 +1166,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="F21">
         <v>98</v>
@@ -1183,16 +1186,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F22">
         <v>36</v>
@@ -1203,16 +1206,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F23">
         <v>37.700000000000003</v>
@@ -1226,7 +1229,7 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
         <v>25</v>
@@ -1235,7 +1238,7 @@
         <v>26</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F25">
         <v>53.6</v>
@@ -1246,16 +1249,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F26">
         <v>58.2</v>
@@ -1266,16 +1269,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F27">
         <v>75.900000000000006</v>
@@ -1286,16 +1289,16 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F28">
         <v>75.400000000000006</v>
@@ -1306,36 +1309,36 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D29" t="s">
         <v>26</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G29">
         <v>88.1</v>
       </c>
       <c r="H29" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D30" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E30" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="F30">
         <v>98</v>
@@ -1346,16 +1349,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D31" t="s">
         <v>26</v>
       </c>
       <c r="E31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F31">
         <v>53.1</v>
@@ -1369,21 +1372,21 @@
         <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C34" t="s">
         <v>25</v>
@@ -1392,7 +1395,7 @@
         <v>26</v>
       </c>
       <c r="E34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F34">
         <v>70.599999999999994</v>
@@ -1403,16 +1406,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C35" t="s">
         <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F35">
         <v>74.2</v>
@@ -1423,7 +1426,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
         <v>25</v>
@@ -1432,7 +1435,7 @@
         <v>26</v>
       </c>
       <c r="E36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F36">
         <v>70</v>
@@ -1443,7 +1446,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="C37" t="s">
         <v>25</v>
@@ -1452,7 +1455,7 @@
         <v>26</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F37">
         <v>69.5</v>
@@ -1463,7 +1466,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
         <v>25</v>
@@ -1472,7 +1475,7 @@
         <v>26</v>
       </c>
       <c r="E38" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F38">
         <v>36.799999999999997</v>
@@ -1483,7 +1486,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C39" t="s">
         <v>25</v>
@@ -1492,7 +1495,7 @@
         <v>26</v>
       </c>
       <c r="E39" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F39">
         <v>47.7</v>
@@ -1503,36 +1506,36 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
         <v>26</v>
       </c>
       <c r="E40" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G40">
         <v>97.2</v>
       </c>
       <c r="H40" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D41" t="s">
         <v>26</v>
       </c>
       <c r="E41" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F41">
         <v>61.2</v>
@@ -1543,16 +1546,16 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" t="s">
         <v>116</v>
       </c>
-      <c r="C42" t="s">
-        <v>130</v>
-      </c>
       <c r="D42" t="s">
         <v>26</v>
       </c>
       <c r="E42" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F42">
         <v>79.3</v>
@@ -1563,16 +1566,16 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C43" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D43" t="s">
         <v>26</v>
       </c>
       <c r="E43" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F43">
         <v>26</v>
@@ -1583,16 +1586,16 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C44" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D44" t="s">
         <v>26</v>
       </c>
       <c r="E44" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F44">
         <v>35.5</v>
@@ -1603,16 +1606,16 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C45" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D45" t="s">
         <v>26</v>
       </c>
       <c r="E45" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F45">
         <v>11.5</v>
@@ -1623,16 +1626,16 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D46" t="s">
         <v>26</v>
       </c>
       <c r="E46" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F46">
         <v>19.100000000000001</v>
@@ -1646,16 +1649,16 @@
         <v>19</v>
       </c>
       <c r="B48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" t="s">
         <v>30</v>
-      </c>
-      <c r="C48" t="s">
-        <v>25</v>
-      </c>
-      <c r="D48" t="s">
-        <v>26</v>
-      </c>
-      <c r="E48" t="s">
-        <v>31</v>
       </c>
       <c r="F48">
         <v>73.7</v>
@@ -1666,7 +1669,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="C49" t="s">
         <v>25</v>
@@ -1675,7 +1678,7 @@
         <v>26</v>
       </c>
       <c r="E49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F49">
         <v>68.400000000000006</v>
@@ -1686,7 +1689,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
       <c r="C50" t="s">
         <v>25</v>
@@ -1695,7 +1698,7 @@
         <v>26</v>
       </c>
       <c r="E50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F50">
         <v>66.400000000000006</v>
@@ -1706,7 +1709,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="C51" t="s">
         <v>25</v>
@@ -1715,7 +1718,7 @@
         <v>26</v>
       </c>
       <c r="E51" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F51">
         <v>49.5</v>
@@ -1726,7 +1729,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="C52" t="s">
         <v>25</v>
@@ -1735,7 +1738,7 @@
         <v>26</v>
       </c>
       <c r="E52" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F52">
         <v>49.5</v>
@@ -1749,16 +1752,16 @@
         <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C54" t="s">
         <v>25</v>
       </c>
       <c r="D54" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E54" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F54">
         <v>70</v>
@@ -1769,16 +1772,16 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C55" t="s">
         <v>25</v>
       </c>
       <c r="D55" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E55" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F55">
         <v>70.3</v>
@@ -1789,16 +1792,16 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C56" t="s">
         <v>25</v>
       </c>
       <c r="D56" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E56" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F56">
         <v>70.3</v>
@@ -1809,7 +1812,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C57" t="s">
         <v>25</v>
@@ -1818,7 +1821,7 @@
         <v>26</v>
       </c>
       <c r="E57" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F57">
         <v>74.2</v>
@@ -1829,7 +1832,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
         <v>25</v>
@@ -1838,7 +1841,7 @@
         <v>26</v>
       </c>
       <c r="E58" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F58">
         <v>74.400000000000006</v>
@@ -1849,7 +1852,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C59" t="s">
         <v>25</v>
@@ -1858,7 +1861,7 @@
         <v>26</v>
       </c>
       <c r="E59" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F59">
         <v>74.2</v>
@@ -1869,16 +1872,16 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C60" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D60" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E60" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F60">
         <v>91.4</v>
@@ -1889,16 +1892,16 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C61" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D61" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E61" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="F61">
         <v>93.3</v>
@@ -1909,16 +1912,16 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C62" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D62" t="s">
         <v>26</v>
       </c>
       <c r="E62" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="F62">
         <v>64.900000000000006</v>
@@ -1929,16 +1932,16 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D63" t="s">
         <v>26</v>
       </c>
       <c r="E63" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="F63">
         <v>10.5</v>
@@ -1952,16 +1955,16 @@
         <v>21</v>
       </c>
       <c r="B65" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C65" t="s">
         <v>25</v>
       </c>
       <c r="D65" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E65" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F65">
         <v>54.8</v>
@@ -1972,16 +1975,16 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C66" t="s">
         <v>25</v>
       </c>
       <c r="D66" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E66" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="F66">
         <v>61.9</v>
@@ -1992,16 +1995,16 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C67" t="s">
         <v>25</v>
       </c>
       <c r="D67" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E67" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="F67">
         <v>61.9</v>
@@ -2012,16 +2015,16 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C68" t="s">
         <v>25</v>
       </c>
       <c r="D68" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E68" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F68">
         <v>77</v>
@@ -2029,19 +2032,22 @@
       <c r="G68">
         <v>94.3</v>
       </c>
+      <c r="H68" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C69" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D69" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E69" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F69">
         <v>77.8</v>
@@ -2055,42 +2061,42 @@
         <v>22</v>
       </c>
       <c r="B71" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C71" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D71" t="s">
         <v>26</v>
       </c>
       <c r="E71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F71" t="s">
         <v>73</v>
       </c>
-      <c r="F71" t="s">
-        <v>86</v>
-      </c>
       <c r="H71" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
+        <v>62</v>
+      </c>
+      <c r="C72" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" t="s">
+        <v>61</v>
+      </c>
+      <c r="F72" t="s">
         <v>74</v>
       </c>
-      <c r="C72" t="s">
-        <v>75</v>
-      </c>
-      <c r="D72" t="s">
-        <v>26</v>
-      </c>
-      <c r="E72" t="s">
-        <v>73</v>
-      </c>
-      <c r="F72" t="s">
-        <v>87</v>
-      </c>
       <c r="H72" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2115,7 +2121,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="C74" t="s">
         <v>25</v>
@@ -2135,7 +2141,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C75" t="s">
         <v>25</v>
@@ -2144,7 +2150,7 @@
         <v>26</v>
       </c>
       <c r="E75" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F75">
         <v>60.6</v>
@@ -2155,7 +2161,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="C76" t="s">
         <v>25</v>
@@ -2164,7 +2170,7 @@
         <v>26</v>
       </c>
       <c r="E76" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F76">
         <v>66.7</v>
@@ -2175,7 +2181,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="C77" t="s">
         <v>25</v>
@@ -2184,7 +2190,7 @@
         <v>26</v>
       </c>
       <c r="E77" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F77">
         <v>60.3</v>
@@ -2195,7 +2201,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="C78" t="s">
         <v>25</v>
@@ -2204,7 +2210,7 @@
         <v>26</v>
       </c>
       <c r="E78" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F78">
         <v>44.7</v>
@@ -2215,16 +2221,16 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="C79" t="s">
         <v>25</v>
       </c>
       <c r="D79" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E79" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="F79">
         <v>62.3</v>
@@ -2235,16 +2241,16 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C80" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D80" t="s">
         <v>26</v>
       </c>
       <c r="E80" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F80">
         <v>31.8</v>
@@ -2255,16 +2261,16 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C81" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D81" t="s">
         <v>26</v>
       </c>
       <c r="E81" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F81">
         <v>14.6</v>
@@ -2275,16 +2281,16 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C82" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D82" t="s">
         <v>26</v>
       </c>
       <c r="E82" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F82">
         <v>7.2</v>
@@ -2295,16 +2301,16 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C83" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D83" t="s">
         <v>26</v>
       </c>
       <c r="E83" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F83">
         <v>1.9</v>
@@ -2315,16 +2321,16 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C84" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D84" t="s">
         <v>26</v>
       </c>
       <c r="E84" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F84">
         <v>27.5</v>
@@ -2335,16 +2341,16 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C85" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D85" t="s">
         <v>26</v>
       </c>
       <c r="E85" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F85">
         <v>42.4</v>
@@ -2378,16 +2384,16 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C88" t="s">
         <v>25</v>
       </c>
       <c r="D88" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E88" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F88">
         <v>67.7</v>
@@ -2398,7 +2404,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>63</v>
+        <v>129</v>
       </c>
       <c r="C89" t="s">
         <v>25</v>
@@ -2407,7 +2413,7 @@
         <v>26</v>
       </c>
       <c r="E89" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F89">
         <v>52.7</v>
@@ -2418,7 +2424,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C90" t="s">
         <v>25</v>
@@ -2427,7 +2433,7 @@
         <v>26</v>
       </c>
       <c r="E90" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F90">
         <v>48.4</v>
@@ -2438,7 +2444,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="C91" t="s">
         <v>25</v>
@@ -2447,7 +2453,7 @@
         <v>26</v>
       </c>
       <c r="E91" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F91">
         <v>42.6</v>
@@ -2458,16 +2464,16 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C92" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D92" t="s">
         <v>26</v>
       </c>
       <c r="E92" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F92">
         <v>25.3</v>
@@ -2478,16 +2484,16 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C93" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D93" t="s">
         <v>26</v>
       </c>
       <c r="E93" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F93">
         <v>46.5</v>
@@ -2498,16 +2504,16 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C94" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D94" t="s">
         <v>26</v>
       </c>
       <c r="E94" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F94">
         <v>33.9</v>

</xml_diff>

<commit_message>
Updated and saved to db World Bank indicators
</commit_message>
<xml_diff>
--- a/Data/Cataloged_Indicators.xlsx
+++ b/Data/Cataloged_Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639FDB92-8CDA-47B0-9D08-D932B2906680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35072DD4-0926-4FC5-BCC2-98D960277952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="536" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="128">
   <si>
     <t>Category</t>
   </si>
@@ -236,15 +236,6 @@
     <t>Current Prices, constant PPPs,  (US Dollar, Million, 2015)</t>
   </si>
   <si>
-    <t>Unemployment Growth QoQ</t>
-  </si>
-  <si>
-    <t>IMF</t>
-  </si>
-  <si>
-    <t>Unemployment Growth YoY</t>
-  </si>
-  <si>
     <t>OECD, Trading Economics, FX Empire</t>
   </si>
   <si>
@@ -287,42 +278,21 @@
     <t>World Bank</t>
   </si>
   <si>
-    <t>GDP per Capita Current US Dollars</t>
-  </si>
-  <si>
     <t>Current US Dollar</t>
   </si>
   <si>
     <t>Population</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>Stock Market Cap</t>
   </si>
   <si>
     <t>Current US Dollars</t>
   </si>
   <si>
-    <t>Listed domestic companies total</t>
-  </si>
-  <si>
     <t>Stock Market Cap Pct of GDP</t>
   </si>
   <si>
-    <t>Stocks traded total value</t>
-  </si>
-  <si>
-    <t>Stocks traded total value Pct of GDP</t>
-  </si>
-  <si>
-    <t>Current account balance</t>
-  </si>
-  <si>
-    <t>Current account balance US Dollars</t>
-  </si>
-  <si>
     <t>Government Expense</t>
   </si>
   <si>
@@ -432,6 +402,24 @@
   </si>
   <si>
     <t>Calculated</t>
+  </si>
+  <si>
+    <t>Listed Domestic Companies Total</t>
+  </si>
+  <si>
+    <t>Stocks Traded Total Value</t>
+  </si>
+  <si>
+    <t>Stocks Traded Total Value Pct of GDP</t>
+  </si>
+  <si>
+    <t>GDP</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Current Account Pct of GDP</t>
   </si>
 </sst>
 </file>
@@ -792,7 +780,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BB27A9-49EB-4C78-B689-287C0457C2BE}">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -828,10 +816,10 @@
         <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -851,7 +839,7 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -865,7 +853,7 @@
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -903,16 +891,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F7">
         <v>76.2</v>
@@ -923,10 +911,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
         <v>46</v>
@@ -943,16 +931,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="F9">
         <v>80.5</v>
@@ -963,16 +951,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F10">
         <v>78.2</v>
@@ -983,10 +971,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D11" t="s">
         <v>46</v>
@@ -1046,7 +1034,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
@@ -1066,7 +1054,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
@@ -1075,7 +1063,7 @@
         <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F16">
         <v>77</v>
@@ -1109,7 +1097,7 @@
         <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
         <v>32</v>
@@ -1121,7 +1109,7 @@
         <v>99.9</v>
       </c>
       <c r="H18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1129,7 +1117,7 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
         <v>32</v>
@@ -1141,21 +1129,21 @@
         <v>99.3</v>
       </c>
       <c r="H19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s">
         <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F20">
         <v>98</v>
@@ -1166,16 +1154,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F21">
         <v>98</v>
@@ -1186,10 +1174,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
         <v>32</v>
@@ -1206,10 +1194,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D23" t="s">
         <v>32</v>
@@ -1269,42 +1257,42 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
         <v>66</v>
       </c>
-      <c r="C27" t="s">
-        <v>67</v>
-      </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27">
-        <v>75.900000000000006</v>
+        <v>30</v>
       </c>
       <c r="G27">
-        <v>84.5</v>
+        <v>88.1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="F28">
-        <v>75.400000000000006</v>
+        <v>98</v>
       </c>
       <c r="G28">
-        <v>83</v>
+        <v>96.7</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1312,7 +1300,7 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="D29" t="s">
         <v>26</v>
@@ -1320,73 +1308,73 @@
       <c r="E29" t="s">
         <v>30</v>
       </c>
+      <c r="F29">
+        <v>53.1</v>
+      </c>
       <c r="G29">
-        <v>88.1</v>
-      </c>
-      <c r="H29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30">
-        <v>98</v>
-      </c>
-      <c r="G30">
-        <v>96.7</v>
+        <v>64.2</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>59</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="E31" t="s">
         <v>30</v>
       </c>
-      <c r="F31">
-        <v>53.1</v>
-      </c>
-      <c r="G31">
-        <v>64.2</v>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="G32">
+        <v>91.1</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E33" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="F33">
+        <v>74.2</v>
+      </c>
+      <c r="G33">
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
         <v>25</v>
@@ -1395,38 +1383,38 @@
         <v>26</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F34">
-        <v>70.599999999999994</v>
+        <v>70</v>
       </c>
       <c r="G34">
-        <v>91.1</v>
+        <v>90.3</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
       <c r="C35" t="s">
         <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E35" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F35">
-        <v>74.2</v>
+        <v>69.5</v>
       </c>
       <c r="G35">
-        <v>94</v>
+        <v>88.2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
         <v>25</v>
@@ -1435,18 +1423,18 @@
         <v>26</v>
       </c>
       <c r="E36" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="F36">
-        <v>70</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="G36">
-        <v>90.3</v>
+        <v>41.8</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>119</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
         <v>25</v>
@@ -1458,58 +1446,58 @@
         <v>48</v>
       </c>
       <c r="F37">
-        <v>69.5</v>
+        <v>47.7</v>
       </c>
       <c r="G37">
-        <v>88.2</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="D38" t="s">
         <v>26</v>
       </c>
       <c r="E38" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38">
-        <v>36.799999999999997</v>
+        <v>34</v>
       </c>
       <c r="G38">
-        <v>41.8</v>
+        <v>97.2</v>
+      </c>
+      <c r="H38" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="C39" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="D39" t="s">
         <v>26</v>
       </c>
       <c r="E39" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F39">
-        <v>47.7</v>
+        <v>61.2</v>
       </c>
       <c r="G39">
-        <v>52.5</v>
+        <v>79.099999999999994</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="D40" t="s">
         <v>26</v>
@@ -1517,19 +1505,19 @@
       <c r="E40" t="s">
         <v>34</v>
       </c>
+      <c r="F40">
+        <v>79.3</v>
+      </c>
       <c r="G40">
-        <v>97.2</v>
-      </c>
-      <c r="H40" t="s">
-        <v>72</v>
+        <v>85.1</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D41" t="s">
         <v>26</v>
@@ -1538,18 +1526,18 @@
         <v>36</v>
       </c>
       <c r="F41">
-        <v>61.2</v>
+        <v>26</v>
       </c>
       <c r="G41">
-        <v>79.099999999999994</v>
+        <v>39.700000000000003</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C42" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D42" t="s">
         <v>26</v>
@@ -1558,18 +1546,18 @@
         <v>34</v>
       </c>
       <c r="F42">
-        <v>79.3</v>
+        <v>35.5</v>
       </c>
       <c r="G42">
-        <v>85.1</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D43" t="s">
         <v>26</v>
@@ -1578,18 +1566,18 @@
         <v>36</v>
       </c>
       <c r="F43">
-        <v>26</v>
+        <v>11.5</v>
       </c>
       <c r="G43">
-        <v>39.700000000000003</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D44" t="s">
         <v>26</v>
@@ -1598,58 +1586,58 @@
         <v>34</v>
       </c>
       <c r="F44">
-        <v>35.5</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="G44">
-        <v>49.5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>113</v>
-      </c>
-      <c r="C45" t="s">
-        <v>116</v>
-      </c>
-      <c r="D45" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" t="s">
-        <v>36</v>
-      </c>
-      <c r="F45">
-        <v>11.5</v>
-      </c>
-      <c r="G45">
-        <v>14.4</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="D46" t="s">
         <v>26</v>
       </c>
       <c r="E46" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F46">
-        <v>19.100000000000001</v>
+        <v>73.7</v>
       </c>
       <c r="G46">
-        <v>19.399999999999999</v>
+        <v>88.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" t="s">
+        <v>30</v>
+      </c>
+      <c r="F47">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="G47">
+        <v>82.6</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="B48" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="C48" t="s">
         <v>25</v>
@@ -1661,15 +1649,15 @@
         <v>30</v>
       </c>
       <c r="F48">
-        <v>73.7</v>
+        <v>66.400000000000006</v>
       </c>
       <c r="G48">
-        <v>88.7</v>
+        <v>83.6</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C49" t="s">
         <v>25</v>
@@ -1678,18 +1666,18 @@
         <v>26</v>
       </c>
       <c r="E49" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F49">
-        <v>68.400000000000006</v>
+        <v>49.5</v>
       </c>
       <c r="G49">
-        <v>82.6</v>
+        <v>62.9</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C50" t="s">
         <v>25</v>
@@ -1698,61 +1686,61 @@
         <v>26</v>
       </c>
       <c r="E50" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F50">
-        <v>66.400000000000006</v>
+        <v>49.5</v>
       </c>
       <c r="G50">
-        <v>83.6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>122</v>
-      </c>
-      <c r="C51" t="s">
-        <v>25</v>
-      </c>
-      <c r="D51" t="s">
-        <v>26</v>
-      </c>
-      <c r="E51" t="s">
-        <v>51</v>
-      </c>
-      <c r="F51">
-        <v>49.5</v>
-      </c>
-      <c r="G51">
         <v>62.9</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B52" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="C52" t="s">
         <v>25</v>
       </c>
       <c r="D52" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E52" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F52">
-        <v>49.5</v>
+        <v>70</v>
       </c>
       <c r="G52">
-        <v>62.9</v>
+        <v>94.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" t="s">
+        <v>34</v>
+      </c>
+      <c r="F53">
+        <v>70.3</v>
+      </c>
+      <c r="G53">
+        <v>89.1</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C54" t="s">
         <v>25</v>
@@ -1761,58 +1749,58 @@
         <v>32</v>
       </c>
       <c r="E54" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F54">
-        <v>70</v>
+        <v>70.3</v>
       </c>
       <c r="G54">
-        <v>94.4</v>
+        <v>89.1</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C55" t="s">
         <v>25</v>
       </c>
       <c r="D55" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E55" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="F55">
-        <v>70.3</v>
+        <v>74.2</v>
       </c>
       <c r="G55">
-        <v>89.1</v>
+        <v>94.6</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s">
         <v>25</v>
       </c>
       <c r="D56" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E56" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="F56">
-        <v>70.3</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="G56">
-        <v>89.1</v>
+        <v>95.3</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C57" t="s">
         <v>25</v>
@@ -1832,130 +1820,130 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
       <c r="C58" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="D58" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E58" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F58">
-        <v>74.400000000000006</v>
+        <v>91.4</v>
       </c>
       <c r="G58">
-        <v>95.3</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="C59" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="D59" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E59" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="F59">
-        <v>74.2</v>
+        <v>93.3</v>
       </c>
       <c r="G59">
-        <v>94.6</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C60" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="D60" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E60" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="F60">
-        <v>91.4</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="G60">
-        <v>96.3</v>
+        <v>81.3</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C61" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="D61" t="s">
+        <v>26</v>
+      </c>
+      <c r="E61" t="s">
+        <v>100</v>
+      </c>
+      <c r="F61">
+        <v>10.5</v>
+      </c>
+      <c r="G61">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" t="s">
         <v>46</v>
       </c>
-      <c r="E61" t="s">
-        <v>88</v>
-      </c>
-      <c r="F61">
-        <v>93.3</v>
-      </c>
-      <c r="G61">
-        <v>96.3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>109</v>
-      </c>
-      <c r="C62" t="s">
-        <v>116</v>
-      </c>
-      <c r="D62" t="s">
-        <v>26</v>
-      </c>
-      <c r="E62" t="s">
-        <v>110</v>
-      </c>
-      <c r="F62">
-        <v>64.900000000000006</v>
-      </c>
-      <c r="G62">
-        <v>81.3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>111</v>
-      </c>
-      <c r="C63" t="s">
-        <v>116</v>
-      </c>
-      <c r="D63" t="s">
-        <v>26</v>
-      </c>
       <c r="E63" t="s">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="F63">
-        <v>10.5</v>
+        <v>54.8</v>
       </c>
       <c r="G63">
-        <v>13.6</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64" t="s">
+        <v>46</v>
+      </c>
+      <c r="E64" t="s">
+        <v>76</v>
+      </c>
+      <c r="F64">
+        <v>61.9</v>
+      </c>
+      <c r="G64">
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="B65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C65" t="s">
         <v>25</v>
@@ -1964,18 +1952,18 @@
         <v>46</v>
       </c>
       <c r="E65" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="F65">
-        <v>54.8</v>
+        <v>61.9</v>
       </c>
       <c r="G65">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C66" t="s">
         <v>25</v>
@@ -1984,124 +1972,124 @@
         <v>46</v>
       </c>
       <c r="E66" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="F66">
-        <v>61.9</v>
+        <v>77</v>
       </c>
       <c r="G66">
-        <v>76</v>
+        <v>94.3</v>
+      </c>
+      <c r="H66" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C67" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="D67" t="s">
         <v>46</v>
       </c>
       <c r="E67" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="F67">
-        <v>61.9</v>
+        <v>77.8</v>
       </c>
       <c r="G67">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>78</v>
-      </c>
-      <c r="C68" t="s">
-        <v>25</v>
-      </c>
-      <c r="D68" t="s">
-        <v>46</v>
-      </c>
-      <c r="E68" t="s">
-        <v>38</v>
-      </c>
-      <c r="F68">
-        <v>77</v>
-      </c>
-      <c r="G68">
-        <v>94.3</v>
-      </c>
-      <c r="H68" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B69" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="C69" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D69" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E69" t="s">
-        <v>38</v>
-      </c>
-      <c r="F69">
-        <v>77.8</v>
-      </c>
-      <c r="G69">
-        <v>81</v>
+        <v>61</v>
+      </c>
+      <c r="F69" t="s">
+        <v>70</v>
+      </c>
+      <c r="H69" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C70" t="s">
+        <v>63</v>
+      </c>
+      <c r="D70" t="s">
+        <v>26</v>
+      </c>
+      <c r="E70" t="s">
+        <v>61</v>
+      </c>
+      <c r="F70" t="s">
+        <v>71</v>
+      </c>
+      <c r="H70" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="B71" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C71" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="D71" t="s">
         <v>26</v>
       </c>
       <c r="E71" t="s">
-        <v>61</v>
-      </c>
-      <c r="F71" t="s">
-        <v>73</v>
-      </c>
-      <c r="H71" t="s">
-        <v>70</v>
+        <v>27</v>
+      </c>
+      <c r="F71">
+        <v>72.7</v>
+      </c>
+      <c r="G71">
+        <v>88.5</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="C72" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="D72" t="s">
         <v>26</v>
       </c>
       <c r="E72" t="s">
-        <v>61</v>
-      </c>
-      <c r="F72" t="s">
-        <v>74</v>
-      </c>
-      <c r="H72" t="s">
-        <v>71</v>
+        <v>27</v>
+      </c>
+      <c r="F72">
+        <v>34</v>
+      </c>
+      <c r="G72">
+        <v>56.7</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C73" t="s">
         <v>25</v>
@@ -2110,18 +2098,18 @@
         <v>26</v>
       </c>
       <c r="E73" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F73">
-        <v>72.7</v>
+        <v>60.6</v>
       </c>
       <c r="G73">
-        <v>88.5</v>
+        <v>72.099999999999994</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C74" t="s">
         <v>25</v>
@@ -2130,18 +2118,18 @@
         <v>26</v>
       </c>
       <c r="E74" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="F74">
-        <v>34</v>
+        <v>66.7</v>
       </c>
       <c r="G74">
-        <v>56.7</v>
+        <v>82.1</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="C75" t="s">
         <v>25</v>
@@ -2150,18 +2138,18 @@
         <v>26</v>
       </c>
       <c r="E75" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="F75">
-        <v>60.6</v>
+        <v>60.3</v>
       </c>
       <c r="G75">
-        <v>72.099999999999994</v>
+        <v>70.5</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C76" t="s">
         <v>25</v>
@@ -2173,78 +2161,78 @@
         <v>56</v>
       </c>
       <c r="F76">
-        <v>66.7</v>
+        <v>44.7</v>
       </c>
       <c r="G76">
-        <v>82.1</v>
+        <v>56.4</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C77" t="s">
         <v>25</v>
       </c>
       <c r="D77" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E77" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="F77">
-        <v>60.3</v>
+        <v>62.3</v>
       </c>
       <c r="G77">
-        <v>70.5</v>
+        <v>82.6</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="C78" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="D78" t="s">
         <v>26</v>
       </c>
       <c r="E78" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F78">
-        <v>44.7</v>
+        <v>31.8</v>
       </c>
       <c r="G78">
-        <v>56.4</v>
+        <v>77.099999999999994</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>128</v>
+        <v>62</v>
       </c>
       <c r="C79" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="D79" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E79" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="F79">
-        <v>62.3</v>
+        <v>14.6</v>
       </c>
       <c r="G79">
-        <v>82.6</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="C80" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D80" t="s">
         <v>26</v>
@@ -2253,18 +2241,18 @@
         <v>61</v>
       </c>
       <c r="F80">
-        <v>31.8</v>
+        <v>7.2</v>
       </c>
       <c r="G80">
-        <v>77.099999999999994</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="C81" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D81" t="s">
         <v>26</v>
@@ -2273,98 +2261,98 @@
         <v>61</v>
       </c>
       <c r="F81">
-        <v>14.6</v>
+        <v>1.9</v>
       </c>
       <c r="G81">
-        <v>42.5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C82" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D82" t="s">
         <v>26</v>
       </c>
       <c r="E82" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="F82">
-        <v>7.2</v>
+        <v>27.5</v>
       </c>
       <c r="G82">
-        <v>19.600000000000001</v>
+        <v>35.799999999999997</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C83" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D83" t="s">
         <v>26</v>
       </c>
       <c r="E83" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="F83">
-        <v>1.9</v>
+        <v>42.4</v>
       </c>
       <c r="G83">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>103</v>
-      </c>
-      <c r="C84" t="s">
-        <v>116</v>
-      </c>
-      <c r="D84" t="s">
-        <v>26</v>
-      </c>
-      <c r="E84" t="s">
-        <v>36</v>
-      </c>
-      <c r="F84">
-        <v>27.5</v>
-      </c>
-      <c r="G84">
-        <v>35.799999999999997</v>
+        <v>50.3</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B85" t="s">
-        <v>104</v>
+        <v>28</v>
       </c>
       <c r="C85" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="D85" t="s">
         <v>26</v>
       </c>
       <c r="E85" t="s">
+        <v>27</v>
+      </c>
+      <c r="F85">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="G85">
+        <v>81.8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>40</v>
+      </c>
+      <c r="C86" t="s">
+        <v>25</v>
+      </c>
+      <c r="D86" t="s">
+        <v>32</v>
+      </c>
+      <c r="E86" t="s">
         <v>34</v>
       </c>
-      <c r="F85">
-        <v>42.4</v>
-      </c>
-      <c r="G85">
-        <v>50.3</v>
+      <c r="F86">
+        <v>67.7</v>
+      </c>
+      <c r="G86">
+        <v>85.9</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="B87" t="s">
-        <v>28</v>
+        <v>119</v>
       </c>
       <c r="C87" t="s">
         <v>25</v>
@@ -2373,38 +2361,38 @@
         <v>26</v>
       </c>
       <c r="E87" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="F87">
-        <v>66.099999999999994</v>
+        <v>52.7</v>
       </c>
       <c r="G87">
-        <v>81.8</v>
+        <v>59.8</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C88" t="s">
         <v>25</v>
       </c>
       <c r="D88" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E88" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="F88">
-        <v>67.7</v>
+        <v>48.4</v>
       </c>
       <c r="G88">
-        <v>85.9</v>
+        <v>53.3</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C89" t="s">
         <v>25</v>
@@ -2416,50 +2404,50 @@
         <v>56</v>
       </c>
       <c r="F89">
-        <v>52.7</v>
+        <v>42.6</v>
       </c>
       <c r="G89">
-        <v>59.8</v>
+        <v>41.8</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="C90" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="D90" t="s">
         <v>26</v>
       </c>
       <c r="E90" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="F90">
-        <v>48.4</v>
+        <v>25.3</v>
       </c>
       <c r="G90">
-        <v>53.3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="C91" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="D91" t="s">
         <v>26</v>
       </c>
       <c r="E91" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="F91">
-        <v>42.6</v>
+        <v>46.5</v>
       </c>
       <c r="G91">
-        <v>41.8</v>
+        <v>55.1</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -2467,58 +2455,18 @@
         <v>105</v>
       </c>
       <c r="C92" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D92" t="s">
         <v>26</v>
       </c>
       <c r="E92" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="F92">
-        <v>25.3</v>
+        <v>33.9</v>
       </c>
       <c r="G92">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>106</v>
-      </c>
-      <c r="C93" t="s">
-        <v>116</v>
-      </c>
-      <c r="D93" t="s">
-        <v>26</v>
-      </c>
-      <c r="E93" t="s">
-        <v>34</v>
-      </c>
-      <c r="F93">
-        <v>46.5</v>
-      </c>
-      <c r="G93">
-        <v>55.1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>115</v>
-      </c>
-      <c r="C94" t="s">
-        <v>116</v>
-      </c>
-      <c r="D94" t="s">
-        <v>26</v>
-      </c>
-      <c r="E94" t="s">
-        <v>61</v>
-      </c>
-      <c r="F94">
-        <v>33.9</v>
-      </c>
-      <c r="G94">
         <v>44.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
backtested models with additional indicators
</commit_message>
<xml_diff>
--- a/Data/Cataloged_Indicators.xlsx
+++ b/Data/Cataloged_Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87255DF5-203E-4ED0-ADD1-D43EB6E62EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DB1753-D87B-4967-A64F-EEE7B0C38FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="536" xr2:uid="{B02CCC66-2C8B-4BB5-8D2A-3F64E1E22706}"/>
   </bookViews>
@@ -777,8 +777,8 @@
   <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H63" sqref="H63"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>